<commit_message>
New Phenology driving oats of photperiod at 4/6 leaf
</commit_message>
<xml_diff>
--- a/Prototypes/Oats/Observed/SowingDateOns.xlsx
+++ b/Prototypes/Oats/Observed/SowingDateOns.xlsx
@@ -89,33 +89,6 @@
     <t>SowingDate2004SowHokSep</t>
   </si>
   <si>
-    <t>SowingDate2002SowDrumMar</t>
-  </si>
-  <si>
-    <t>SowingDate2002SowDrumMay</t>
-  </si>
-  <si>
-    <t>SowingDate2002SowDrumSep</t>
-  </si>
-  <si>
-    <t>SowingDate2003SowDrumMar</t>
-  </si>
-  <si>
-    <t>SowingDate2003SowDrumMay</t>
-  </si>
-  <si>
-    <t>SowingDate2003SowDrumSep</t>
-  </si>
-  <si>
-    <t>SowingDate2004SowDrumMar</t>
-  </si>
-  <si>
-    <t>SowingDate2004SowDrumMay</t>
-  </si>
-  <si>
-    <t>SowingDate2004SowDrumSep</t>
-  </si>
-  <si>
     <t>Sow</t>
   </si>
   <si>
@@ -128,16 +101,43 @@
     <t>HokSep</t>
   </si>
   <si>
-    <t>DrumMar</t>
-  </si>
-  <si>
-    <t>DrumMay</t>
-  </si>
-  <si>
-    <t>DrumSep</t>
-  </si>
-  <si>
     <t>Oats.Structure.MainStemFinalNodeNumber</t>
+  </si>
+  <si>
+    <t>SowingDate2002SowStamMar</t>
+  </si>
+  <si>
+    <t>StamMar</t>
+  </si>
+  <si>
+    <t>SowingDate2002SowStamMay</t>
+  </si>
+  <si>
+    <t>StamMay</t>
+  </si>
+  <si>
+    <t>SowingDate2002SowStamSep</t>
+  </si>
+  <si>
+    <t>StamSep</t>
+  </si>
+  <si>
+    <t>SowingDate2003SowStamMar</t>
+  </si>
+  <si>
+    <t>SowingDate2003SowStamMay</t>
+  </si>
+  <si>
+    <t>SowingDate2003SowStamSep</t>
+  </si>
+  <si>
+    <t>SowingDate2004SowStamMar</t>
+  </si>
+  <si>
+    <t>SowingDate2004SowStamMay</t>
+  </si>
+  <si>
+    <t>SowingDate2004SowStamSep</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E9:E10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -527,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>246</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>197</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>104</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>236</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>190</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>115</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>229</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>184</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>116</v>
       </c>
       <c r="L10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
@@ -927,7 +927,7 @@
         <v>242</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
@@ -967,7 +967,7 @@
         <v>182</v>
       </c>
       <c r="L12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
@@ -1007,7 +1007,7 @@
         <v>94</v>
       </c>
       <c r="L13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
@@ -1047,7 +1047,7 @@
         <v>231</v>
       </c>
       <c r="L14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
@@ -1087,7 +1087,7 @@
         <v>181</v>
       </c>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
@@ -1127,7 +1127,7 @@
         <v>103</v>
       </c>
       <c r="L16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1156,18 +1156,18 @@
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>203</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+      <c r="L17" t="s">
         <v>27</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>203</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="L17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
@@ -1207,7 +1207,7 @@
         <v>172</v>
       </c>
       <c r="L18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
@@ -1247,7 +1247,7 @@
         <v>114</v>
       </c>
       <c r="L19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>